<commit_message>
-added new file impact_factor.py -save impact_factor.png -minor change in exporting loads.xlsx
</commit_message>
<xml_diff>
--- a/outputs/loads.xlsx
+++ b/outputs/loads.xlsx
@@ -455,50 +455,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>6.25</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>18.75</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>25.0</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>31.25</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>37.5</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>43.75</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>50.0</t>
-        </is>
+      <c r="C1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>18.75</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>43.75</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="2">

</xml_diff>